<commit_message>
cambios en asignacion inicial, recotizada, duplicados. Cambio en clase load para incluir posibles tables o schemas
</commit_message>
<xml_diff>
--- a/data/arbol_tipificacion/00.arbol_tipificacion_v2.xlsx
+++ b/data/arbol_tipificacion/00.arbol_tipificacion_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WORKFORCE\03. Mission\Emerson Aguilar\19. Axa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emerson.Aguilar\Documents\git_hub\Axa\data\arbol_tipificacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D91B97-5DEE-4F2A-B50A-C940D8F50AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3E18D3-5F28-4EC0-B265-51F5092615EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{0C8A8193-BE22-47A8-93B6-FEFE6A3FB9E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C8A8193-BE22-47A8-93B6-FEFE6A3FB9E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Consulta1" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
   <si>
     <t>status</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>Otro</t>
+  </si>
+  <si>
+    <t>plataforma</t>
+  </si>
+  <si>
+    <t>vicidial</t>
   </si>
 </sst>
 </file>
@@ -281,7 +287,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -524,21 +549,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AF1B66D0-21EA-45C9-9FFB-D72F8546D969}" name="Tabla1" displayName="Tabla1" ref="A1:J24" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AF1B66D0-21EA-45C9-9FFB-D72F8546D969}" name="Tabla1" displayName="Tabla1" ref="A1:K24" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J24">
     <sortCondition ref="E1:E24"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{B444EE17-F97A-485E-A302-C36903522534}" name="status" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{66866C76-E589-4687-A26C-78F67F137BF3}" name="status_name" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{68A67A4C-6B09-4218-BF9C-964B0FD3773B}" name="tipificacion" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{2CA89C42-67E6-4180-99CF-D396E4721EF2}" name="tipo_contacto" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{5659C2A4-9BB7-4161-8C2B-A6CAF8FD81E5}" name="prioridad" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{A1910C75-997E-4240-862B-06F5885B913E}" name="efectivo" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{E3B887F7-2301-4986-A908-47A48D5F449B}" name="contacto" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{F6F68430-5DD4-4BCC-8FB2-2271934F4C7A}" name="no_contacto" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{75838347-BC15-4373-BDD0-5887B1F3909D}" name="contacto_efectivo" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{C008011B-256C-4E83-89A2-9DEBAF67DDDA}" name="contacto_no_efectivo" dataDxfId="2"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{B444EE17-F97A-485E-A302-C36903522534}" name="status" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{66866C76-E589-4687-A26C-78F67F137BF3}" name="status_name" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{68A67A4C-6B09-4218-BF9C-964B0FD3773B}" name="tipificacion" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{2CA89C42-67E6-4180-99CF-D396E4721EF2}" name="tipo_contacto" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5659C2A4-9BB7-4161-8C2B-A6CAF8FD81E5}" name="prioridad" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{A1910C75-997E-4240-862B-06F5885B913E}" name="efectivo" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{E3B887F7-2301-4986-A908-47A48D5F449B}" name="contacto" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{F6F68430-5DD4-4BCC-8FB2-2271934F4C7A}" name="no_contacto" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{75838347-BC15-4373-BDD0-5887B1F3909D}" name="contacto_efectivo" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{C008011B-256C-4E83-89A2-9DEBAF67DDDA}" name="contacto_no_efectivo" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{F2181076-9505-4340-9592-341A76F8ADB3}" name="plataforma" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -861,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48039E35-E3AF-482A-89BA-59A77FCE3EF8}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -881,7 +907,7 @@
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -912,8 +938,11 @@
       <c r="J1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
@@ -944,8 +973,11 @@
       <c r="J2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -976,8 +1008,11 @@
       <c r="J3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
@@ -1008,8 +1043,11 @@
       <c r="J4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>56</v>
       </c>
@@ -1040,8 +1078,11 @@
       <c r="J5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1072,8 +1113,11 @@
       <c r="J6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1104,8 +1148,11 @@
       <c r="J7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -1136,8 +1183,11 @@
       <c r="J8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
@@ -1168,8 +1218,11 @@
       <c r="J9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1200,8 +1253,11 @@
       <c r="J10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1232,8 +1288,11 @@
       <c r="J11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1264,12 +1323,17 @@
       <c r="J12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
@@ -1294,8 +1358,11 @@
       <c r="J13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1326,8 +1393,11 @@
       <c r="J14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1358,8 +1428,11 @@
       <c r="J15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -1390,8 +1463,11 @@
       <c r="J16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1422,8 +1498,11 @@
       <c r="J17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1454,8 +1533,11 @@
       <c r="J18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1486,8 +1568,11 @@
       <c r="J19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1518,8 +1603,11 @@
       <c r="J20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
@@ -1550,8 +1638,11 @@
       <c r="J21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -1582,12 +1673,17 @@
       <c r="J22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
@@ -1612,12 +1708,17 @@
       <c r="J23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C24" s="1" t="s">
         <v>40</v>
       </c>
@@ -1641,6 +1742,9 @@
       </c>
       <c r="J24" s="1">
         <v>0</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion config formulario and depurador predictivo falabella
</commit_message>
<xml_diff>
--- a/data/arbol_tipificacion/00.arbol_tipificacion_v2.xlsx
+++ b/data/arbol_tipificacion/00.arbol_tipificacion_v2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emerson.Aguilar\Documents\git_hub\Axa\data\arbol_tipificacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3E18D3-5F28-4EC0-B265-51F5092615EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50541275-1E84-4B62-88E0-1102F91BAF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C8A8193-BE22-47A8-93B6-FEFE6A3FB9E1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C8A8193-BE22-47A8-93B6-FEFE6A3FB9E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Consulta1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">Consulta1!$A$1:$J$24</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">Consulta1!$A$1:$J$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="70">
   <si>
     <t>status</t>
   </si>
@@ -233,6 +233,33 @@
   </si>
   <si>
     <t>vicidial</t>
+  </si>
+  <si>
+    <t>SVYCLM</t>
+  </si>
+  <si>
+    <t>Survey sent to Call Menu</t>
+  </si>
+  <si>
+    <t>Blaster - Encuesta enviada a Call Menu</t>
+  </si>
+  <si>
+    <t>Blaster - Contacto</t>
+  </si>
+  <si>
+    <t>Blaster Vicidial</t>
+  </si>
+  <si>
+    <t>PU</t>
+  </si>
+  <si>
+    <t>Call Picked Up</t>
+  </si>
+  <si>
+    <t>Blaster - Llamada atendida</t>
+  </si>
+  <si>
+    <t>ADAIR</t>
   </si>
 </sst>
 </file>
@@ -495,7 +522,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -549,9 +576,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AF1B66D0-21EA-45C9-9FFB-D72F8546D969}" name="Tabla1" displayName="Tabla1" ref="A1:K24" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J24">
-    <sortCondition ref="E1:E24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AF1B66D0-21EA-45C9-9FFB-D72F8546D969}" name="Tabla1" displayName="Tabla1" ref="A1:K27" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J26">
+    <sortCondition ref="E1:E26"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{B444EE17-F97A-485E-A302-C36903522534}" name="status" dataDxfId="10"/>
@@ -887,27 +914,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48039E35-E3AF-482A-89BA-59A77FCE3EF8}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +969,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
@@ -977,7 +1004,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1012,7 +1039,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
@@ -1047,7 +1074,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>56</v>
       </c>
@@ -1082,7 +1109,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1117,7 +1144,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1152,7 +1179,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -1187,7 +1214,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
@@ -1222,18 +1249,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="E10" s="1">
         <v>9</v>
@@ -1242,10 +1269,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1">
         <v>0</v>
@@ -1254,21 +1281,21 @@
         <v>0</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="E11" s="1">
         <v>10</v>
@@ -1277,10 +1304,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
@@ -1289,18 +1316,18 @@
         <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>43</v>
@@ -1327,15 +1354,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>43</v>
@@ -1362,15 +1389,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>43</v>
@@ -1397,15 +1424,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>43</v>
@@ -1432,15 +1459,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>26</v>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>43</v>
@@ -1467,15 +1494,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>11</v>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>43</v>
@@ -1502,15 +1529,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>7</v>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>43</v>
@@ -1537,15 +1564,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>28</v>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>43</v>
@@ -1572,15 +1599,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>9</v>
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>43</v>
@@ -1607,15 +1634,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>50</v>
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>43</v>
@@ -1642,15 +1669,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>5</v>
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>43</v>
@@ -1677,15 +1704,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>3</v>
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>43</v>
@@ -1712,15 +1739,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>17</v>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>43</v>
@@ -1744,6 +1771,111 @@
         <v>0</v>
       </c>
       <c r="K24" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="1">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="1">
+        <v>25</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="1">
+        <v>26</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>